<commit_message>
Pooh Points: normal 20260204
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-04.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-04.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="34" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -1879,83 +1879,83 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Undrafted</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Bishop Boswell</t>
+          <t>Rashaun Agee</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Wed, February 4th at 7:00 PM EST</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1976,17 +1976,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Camden Heide</t>
+          <t>Bishop Boswell</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1995,49 +1995,49 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I19" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J19" t="n">
+        <v>8</v>
+      </c>
+      <c r="K19" t="n">
         <v>5</v>
       </c>
-      <c r="K19" t="n">
-        <v>2</v>
-      </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P19" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q19" t="n">
+        <v>2</v>
+      </c>
+      <c r="R19" t="n">
+        <v>5</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" t="n">
         <v>4</v>
       </c>
-      <c r="R19" t="n">
-        <v>7</v>
-      </c>
-      <c r="S19" t="n">
-        <v>3</v>
-      </c>
-      <c r="T19" t="n">
-        <v>6</v>
-      </c>
       <c r="U19" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V19" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -2058,17 +2058,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Patton Pinkins</t>
+          <t>Camden Heide</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2077,19 +2077,19 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I20" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
@@ -2101,13 +2101,13 @@
         <v>1</v>
       </c>
       <c r="P20" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R20" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S20" t="n">
         <v>3</v>
@@ -2116,7 +2116,7 @@
         <v>6</v>
       </c>
       <c r="U20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V20" t="n">
         <v>2</v>
@@ -2140,17 +2140,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Simeon Wilcher</t>
+          <t>Patton Pinkins</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2159,16 +2159,16 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I21" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2180,22 +2180,22 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P21" t="n">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R21" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T21" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="U21" t="n">
         <v>2</v>
@@ -2222,12 +2222,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>EJ Walker</t>
+          <t>Simeon Wilcher</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2241,16 +2241,16 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L22" t="n">
         <v>1</v>
@@ -2265,25 +2265,25 @@
         <v>4</v>
       </c>
       <c r="P22" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q22" t="n">
+        <v>2</v>
+      </c>
+      <c r="R22" t="n">
         <v>4</v>
       </c>
-      <c r="R22" t="n">
-        <v>5</v>
-      </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Elijah Strong</t>
+          <t>EJ Walker</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2326,7 +2326,7 @@
         <v>10</v>
       </c>
       <c r="I23" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J23" t="n">
         <v>3</v>
@@ -2335,37 +2335,37 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
         <v>4</v>
       </c>
       <c r="P23" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="Q23" t="n">
+        <v>4</v>
+      </c>
+      <c r="R23" t="n">
         <v>5</v>
       </c>
-      <c r="R23" t="n">
-        <v>10</v>
-      </c>
       <c r="S23" t="n">
         <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -2386,17 +2386,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Eduardo Klafke</t>
+          <t>Elijah Strong</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2405,49 +2405,49 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I24" t="n">
+        <v>12</v>
+      </c>
+      <c r="J24" t="n">
+        <v>3</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>4</v>
+      </c>
+      <c r="P24" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>5</v>
+      </c>
+      <c r="R24" t="n">
         <v>10</v>
       </c>
-      <c r="J24" t="n">
-        <v>2</v>
-      </c>
-      <c r="K24" t="n">
-        <v>1</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>3</v>
-      </c>
-      <c r="P24" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>3</v>
-      </c>
-      <c r="R24" t="n">
-        <v>4</v>
-      </c>
       <c r="S24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
         <v>2</v>
       </c>
       <c r="U24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V24" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -2468,17 +2468,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Chendall Weaver</t>
+          <t>Eduardo Klafke</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2487,49 +2487,49 @@
         </is>
       </c>
       <c r="H25" t="n">
+        <v>9</v>
+      </c>
+      <c r="I25" t="n">
+        <v>10</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>3</v>
+      </c>
+      <c r="P25" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>3</v>
+      </c>
+      <c r="R25" t="n">
+        <v>4</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="n">
+        <v>2</v>
+      </c>
+      <c r="U25" t="n">
+        <v>3</v>
+      </c>
+      <c r="V25" t="n">
         <v>6</v>
-      </c>
-      <c r="I25" t="n">
-        <v>5</v>
-      </c>
-      <c r="J25" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>1</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" t="n">
-        <v>3</v>
-      </c>
-      <c r="P25" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>2</v>
-      </c>
-      <c r="R25" t="n">
-        <v>2</v>
-      </c>
-      <c r="S25" t="n">
-        <v>1</v>
-      </c>
-      <c r="T25" t="n">
-        <v>1</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2550,17 +2550,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Augusto Cassiá</t>
+          <t>Chendall Weaver</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2569,49 +2569,49 @@
         </is>
       </c>
       <c r="H26" t="n">
+        <v>6</v>
+      </c>
+      <c r="I26" t="n">
         <v>5</v>
       </c>
-      <c r="I26" t="n">
-        <v>2</v>
-      </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
         <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P26" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Q26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="n">
         <v>0</v>
       </c>
       <c r="V26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2632,12 +2632,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>DeWayne Brown II</t>
+          <t>Augusto Cassiá</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2654,46 +2654,46 @@
         <v>5</v>
       </c>
       <c r="I27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J27" t="n">
+        <v>4</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
         <v>5</v>
       </c>
-      <c r="J27" t="n">
-        <v>3</v>
-      </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N27" t="n">
-        <v>1</v>
-      </c>
-      <c r="O27" t="n">
-        <v>2</v>
-      </c>
       <c r="P27" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Q27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R27" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2714,12 +2714,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Kezza Giffa</t>
+          <t>DeWayne Brown II</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2736,46 +2736,46 @@
         <v>5</v>
       </c>
       <c r="I28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K28" t="n">
         <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P28" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="Q28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R28" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -2796,17 +2796,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Lassina Traore</t>
+          <t>Kezza Giffa</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2818,13 +2818,13 @@
         <v>5</v>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
         <v>0</v>
@@ -2836,28 +2836,28 @@
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2878,17 +2878,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Amari Evans</t>
+          <t>Lassina Traore</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2897,16 +2897,16 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
@@ -2918,10 +2918,10 @@
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P30" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -2933,13 +2933,13 @@
         <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V30" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -2960,12 +2960,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Niko Bundalo</t>
+          <t>Amari Evans</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2985,10 +2985,10 @@
         <v>2</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
         <v>0</v>
@@ -3000,28 +3000,28 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Q31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S31" t="n">
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -3042,12 +3042,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Troy Henderson</t>
+          <t>Niko Bundalo</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3064,13 +3064,13 @@
         <v>3</v>
       </c>
       <c r="I32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" t="n">
         <v>0</v>
@@ -3082,22 +3082,22 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q32" t="n">
         <v>1</v>
       </c>
       <c r="R32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
         <v>0</v>
@@ -3124,12 +3124,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Corey Chest</t>
+          <t>Troy Henderson</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3143,43 +3143,43 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" t="n">
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P33" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U33" t="n">
         <v>0</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Koren Johnson</t>
+          <t>Corey Chest</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3228,25 +3228,25 @@
         <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" t="n">
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P34" t="n">
         <v>11</v>
@@ -3255,19 +3255,19 @@
         <v>0</v>
       </c>
       <c r="R34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
       </c>
       <c r="T34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -3288,17 +3288,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Christ Essandoko</t>
+          <t>Koren Johnson</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3307,16 +3307,16 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
         <v>0</v>
@@ -3325,31 +3325,31 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" t="n">
         <v>2</v>
       </c>
       <c r="P35" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
       <c r="R35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S35" t="n">
         <v>0</v>
       </c>
       <c r="T35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Eli Ellis</t>
+          <t>Christ Essandoko</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -3392,10 +3392,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
         <v>0</v>
@@ -3407,25 +3407,25 @@
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P36" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="Q36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U36" t="n">
         <v>0</v>
@@ -3452,17 +3452,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Ethan Burg</t>
+          <t>Eli Ellis</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3474,10 +3474,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
@@ -3489,25 +3489,25 @@
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U37" t="n">
         <v>0</v>
@@ -3534,17 +3534,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Hayden Assemian</t>
+          <t>Ethan Burg</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>SC@TEX</t>
+          <t>MISS@TENN</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
         <v>1</v>
@@ -3616,17 +3616,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Max Smith</t>
+          <t>Hayden Assemian</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>MISS@TENN</t>
+          <t>SC@TEX</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3656,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P39" t="n">
         <v>1</v>
@@ -3698,12 +3698,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Clarence Massamba</t>
+          <t>Max Smith</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -3738,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40" t="n">
         <v>1</v>
@@ -3747,13 +3747,13 @@
         <v>0</v>
       </c>
       <c r="R40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
       </c>
       <c r="T40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" t="n">
         <v>0</v>
@@ -3780,12 +3780,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Travis Perry</t>
+          <t>Clarence Massamba</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3799,43 +3799,43 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
       </c>
       <c r="N41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41" t="n">
         <v>1</v>
       </c>
       <c r="P41" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
       <c r="R41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S41" t="n">
         <v>0</v>
       </c>
       <c r="T41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U41" t="n">
         <v>0</v>
@@ -3862,67 +3862,149 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t>Travis Perry</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>MISS</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>MISS@TENN</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>-2</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1</v>
+      </c>
+      <c r="P42" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>3</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>3</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>Grant Polk</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>SC</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>SC@TEX</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>Final</t>
         </is>
       </c>
-      <c r="H42" t="n">
+      <c r="H43" t="n">
         <v>-3</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" t="n">
-        <v>1</v>
-      </c>
-      <c r="P42" t="n">
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1</v>
+      </c>
+      <c r="P43" t="n">
         <v>10</v>
       </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="n">
-        <v>3</v>
-      </c>
-      <c r="S42" t="n">
-        <v>0</v>
-      </c>
-      <c r="T42" t="n">
-        <v>1</v>
-      </c>
-      <c r="U42" t="n">
-        <v>0</v>
-      </c>
-      <c r="V42" t="n">
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>3</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4039,10 +4121,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Pooh Points: final 20260204 -> PD10
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-04.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-04.xlsx
@@ -434,7 +434,7 @@
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="34" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -1007,53 +1007,53 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I7" t="n">
+        <v>11</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2</v>
+      </c>
+      <c r="R7" t="n">
         <v>6</v>
       </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>2</v>
-      </c>
-      <c r="R7" t="n">
-        <v>5</v>
-      </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -1417,20 +1417,20 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12" t="n">
         <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -1442,22 +1442,22 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="Q12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" t="n">
+        <v>8</v>
+      </c>
+      <c r="S12" t="n">
+        <v>2</v>
+      </c>
+      <c r="T12" t="n">
         <v>6</v>
-      </c>
-      <c r="S12" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" t="n">
-        <v>4</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -1499,47 +1499,47 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" t="n">
+        <v>8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
         <v>5</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>3</v>
+      </c>
+      <c r="R13" t="n">
+        <v>10</v>
+      </c>
+      <c r="S13" t="n">
+        <v>2</v>
+      </c>
+      <c r="T13" t="n">
         <v>6</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
-        <v>3</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" t="n">
-        <v>1</v>
-      </c>
-      <c r="P13" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>2</v>
-      </c>
-      <c r="R13" t="n">
-        <v>6</v>
-      </c>
-      <c r="S13" t="n">
-        <v>2</v>
-      </c>
-      <c r="T13" t="n">
-        <v>4</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1745,20 +1745,20 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I16" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J16" t="n">
         <v>3</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" t="n">
         <v>1</v>
@@ -1767,31 +1767,31 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" t="n">
         <v>1</v>
       </c>
       <c r="P16" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="Q16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R16" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="S16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T16" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1827,17 +1827,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
         <v>1</v>
@@ -1849,19 +1849,19 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="Q17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -2140,35 +2140,35 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Houston Mallette</t>
+          <t>Otega Oweh</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="I21" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J21" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
@@ -2180,28 +2180,28 @@
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P21" t="n">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="Q21" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R21" t="n">
+        <v>11</v>
+      </c>
+      <c r="S21" t="n">
+        <v>3</v>
+      </c>
+      <c r="T21" t="n">
+        <v>4</v>
+      </c>
+      <c r="U21" t="n">
+        <v>7</v>
+      </c>
+      <c r="V21" t="n">
         <v>9</v>
-      </c>
-      <c r="S21" t="n">
-        <v>4</v>
-      </c>
-      <c r="T21" t="n">
-        <v>8</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2222,35 +2222,35 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Otega Oweh</t>
+          <t>Houston Mallette</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I22" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
@@ -2259,31 +2259,31 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P22" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R22" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T22" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="U22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2468,65 +2468,65 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Amari Allen</t>
+          <t>Xzayvier Brown</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I25" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J25" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K25" t="n">
+        <v>4</v>
+      </c>
+      <c r="L25" t="n">
+        <v>2</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O25" t="n">
+        <v>4</v>
+      </c>
+      <c r="P25" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q25" t="n">
         <v>6</v>
       </c>
-      <c r="L25" t="n">
-        <v>2</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" t="n">
-        <v>3</v>
-      </c>
-      <c r="P25" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>4</v>
-      </c>
       <c r="R25" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T25" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V25" t="n">
         <v>4</v>
@@ -2550,68 +2550,68 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Xzayvier Brown</t>
+          <t>Amari Allen</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H26" t="n">
+        <v>18</v>
+      </c>
+      <c r="I26" t="n">
+        <v>12</v>
+      </c>
+      <c r="J26" t="n">
         <v>7</v>
       </c>
-      <c r="I26" t="n">
-        <v>5</v>
-      </c>
-      <c r="J26" t="n">
-        <v>1</v>
-      </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
         <v>0</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P26" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="Q26" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R26" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T26" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="U26" t="n">
         <v>2</v>
       </c>
       <c r="V26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -2647,14 +2647,14 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J27" t="n">
         <v>2</v>
@@ -2672,10 +2672,10 @@
         <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P27" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
@@ -2690,10 +2690,10 @@
         <v>0</v>
       </c>
       <c r="U27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -2757,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q28" t="n">
         <v>0</v>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -3042,12 +3042,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Mouhamed Dioubate</t>
+          <t>Mohamed Wague</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3057,41 +3057,41 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I32" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P32" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="Q32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -3124,12 +3124,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mohamed Wague</t>
+          <t>Mouhamed Dioubate</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3139,53 +3139,53 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P33" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -3303,17 +3303,17 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -3325,25 +3325,25 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R35" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T35" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U35" t="n">
         <v>0</v>
@@ -3452,41 +3452,41 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Aiden Sherrell</t>
+          <t>Tae Davis</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I37" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J37" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L37" t="n">
         <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
@@ -3495,25 +3495,25 @@
         <v>3</v>
       </c>
       <c r="P37" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R37" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="S37" t="n">
         <v>0</v>
       </c>
       <c r="T37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U37" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V37" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -3534,12 +3534,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Rashaun Agee</t>
+          <t>Aiden Sherrell</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3549,53 +3549,53 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I38" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L38" t="n">
         <v>1</v>
       </c>
       <c r="M38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P38" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="Q38" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R38" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="S38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U38" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V38" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
@@ -3616,41 +3616,41 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Tae Davis</t>
+          <t>Rashaun Agee</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I39" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="J39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -3659,25 +3659,25 @@
         <v>2</v>
       </c>
       <c r="P39" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>7</v>
+      </c>
+      <c r="R39" t="n">
         <v>15</v>
       </c>
-      <c r="Q39" t="n">
-        <v>4</v>
-      </c>
-      <c r="R39" t="n">
-        <v>8</v>
-      </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T39" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V39" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H40" t="n">
@@ -5830,68 +5830,68 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Jamie Vinson</t>
+          <t>Brandon Garrison</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I66" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="J66" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K66" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L66" t="n">
         <v>0</v>
       </c>
       <c r="M66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P66" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>7</v>
+      </c>
+      <c r="R66" t="n">
         <v>8</v>
       </c>
-      <c r="Q66" t="n">
-        <v>4</v>
-      </c>
-      <c r="R66" t="n">
-        <v>5</v>
-      </c>
       <c r="S66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T66" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
@@ -5912,68 +5912,68 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Jacari Lane</t>
+          <t>Andrija Jelavic</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I67" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J67" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K67" t="n">
+        <v>3</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>2</v>
+      </c>
+      <c r="P67" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>3</v>
+      </c>
+      <c r="R67" t="n">
         <v>5</v>
       </c>
-      <c r="L67" t="n">
-        <v>1</v>
-      </c>
-      <c r="M67" t="n">
-        <v>0</v>
-      </c>
-      <c r="N67" t="n">
-        <v>0</v>
-      </c>
-      <c r="O67" t="n">
-        <v>4</v>
-      </c>
-      <c r="P67" t="n">
-        <v>28</v>
-      </c>
-      <c r="Q67" t="n">
-        <v>2</v>
-      </c>
-      <c r="R67" t="n">
-        <v>7</v>
-      </c>
       <c r="S67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T67" t="n">
         <v>3</v>
       </c>
       <c r="U67" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V67" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -5994,7 +5994,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Josh Holloway</t>
+          <t>Jamie Vinson</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6009,53 +6009,53 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H68" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I68" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K68" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O68" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P68" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R68" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S68" t="n">
         <v>1</v>
       </c>
       <c r="T68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U68" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V68" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -6076,12 +6076,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>London Jemison</t>
+          <t>Jacari Lane</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6091,23 +6091,23 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H69" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I69" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K69" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M69" t="n">
         <v>0</v>
@@ -6116,28 +6116,28 @@
         <v>0</v>
       </c>
       <c r="O69" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P69" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="Q69" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R69" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U69" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V69" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -6158,50 +6158,50 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Andrija Jelavic</t>
+          <t>Josh Holloway</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H70" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I70" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" t="n">
         <v>0</v>
       </c>
       <c r="N70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P70" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q70" t="n">
         <v>2</v>
@@ -6210,16 +6210,16 @@
         <v>3</v>
       </c>
       <c r="S70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -6240,12 +6240,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Zach Clemence</t>
+          <t>London Jemison</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6255,53 +6255,53 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H71" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J71" t="n">
+        <v>4</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="n">
+        <v>1</v>
+      </c>
+      <c r="P71" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>4</v>
+      </c>
+      <c r="R71" t="n">
         <v>6</v>
       </c>
-      <c r="J71" t="n">
-        <v>2</v>
-      </c>
-      <c r="K71" t="n">
-        <v>0</v>
-      </c>
-      <c r="L71" t="n">
-        <v>1</v>
-      </c>
-      <c r="M71" t="n">
-        <v>0</v>
-      </c>
-      <c r="N71" t="n">
-        <v>0</v>
-      </c>
-      <c r="O71" t="n">
-        <v>4</v>
-      </c>
-      <c r="P71" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q71" t="n">
-        <v>2</v>
-      </c>
-      <c r="R71" t="n">
-        <v>2</v>
-      </c>
       <c r="S71" t="n">
         <v>2</v>
       </c>
       <c r="T71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U71" t="n">
         <v>0</v>
       </c>
       <c r="V71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -6322,68 +6322,68 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Brandon Garrison</t>
+          <t>Zach Clemence</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H72" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I72" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M72" t="n">
         <v>0</v>
       </c>
       <c r="N72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O72" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P72" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S72" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T72" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -6404,12 +6404,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Dayton Forsythe</t>
+          <t>Jasper Johnson</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6419,20 +6419,20 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I73" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" t="n">
         <v>0</v>
@@ -6444,28 +6444,28 @@
         <v>0</v>
       </c>
       <c r="O73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P73" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="Q73" t="n">
         <v>2</v>
       </c>
       <c r="R73" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S73" t="n">
         <v>1</v>
       </c>
       <c r="T73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U73" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V73" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -6486,35 +6486,35 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Jasper Johnson</t>
+          <t>Pop Isaacs</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>OU@UK</t>
+          <t>TA&amp;M@ALA</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H74" t="n">
         <v>6</v>
       </c>
       <c r="I74" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L74" t="n">
         <v>0</v>
@@ -6523,25 +6523,25 @@
         <v>0</v>
       </c>
       <c r="N74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P74" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R74" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="S74" t="n">
         <v>1</v>
       </c>
       <c r="T74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U74" t="n">
         <v>0</v>
@@ -6568,12 +6568,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Pop Isaacs</t>
+          <t>Charles Bediako</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6583,53 +6583,53 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I75" t="n">
+        <v>5</v>
+      </c>
+      <c r="J75" t="n">
+        <v>4</v>
+      </c>
+      <c r="K75" t="n">
+        <v>1</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="n">
+        <v>1</v>
+      </c>
+      <c r="N75" t="n">
+        <v>1</v>
+      </c>
+      <c r="O75" t="n">
+        <v>2</v>
+      </c>
+      <c r="P75" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>1</v>
+      </c>
+      <c r="R75" t="n">
+        <v>2</v>
+      </c>
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1</v>
+      </c>
+      <c r="U75" t="n">
+        <v>3</v>
+      </c>
+      <c r="V75" t="n">
         <v>7</v>
-      </c>
-      <c r="J75" t="n">
-        <v>4</v>
-      </c>
-      <c r="K75" t="n">
-        <v>2</v>
-      </c>
-      <c r="L75" t="n">
-        <v>0</v>
-      </c>
-      <c r="M75" t="n">
-        <v>0</v>
-      </c>
-      <c r="N75" t="n">
-        <v>1</v>
-      </c>
-      <c r="O75" t="n">
-        <v>1</v>
-      </c>
-      <c r="P75" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q75" t="n">
-        <v>3</v>
-      </c>
-      <c r="R75" t="n">
-        <v>9</v>
-      </c>
-      <c r="S75" t="n">
-        <v>1</v>
-      </c>
-      <c r="T75" t="n">
-        <v>3</v>
-      </c>
-      <c r="U75" t="n">
-        <v>0</v>
-      </c>
-      <c r="V75" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -6650,32 +6650,32 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Charles Bediako</t>
+          <t>Dayton Forsythe</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>TA&amp;M@ALA</t>
+          <t>OU@UK</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H76" t="n">
         <v>5</v>
       </c>
       <c r="I76" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J76" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K76" t="n">
         <v>1</v>
@@ -6684,34 +6684,34 @@
         <v>0</v>
       </c>
       <c r="M76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P76" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R76" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V76" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -6747,7 +6747,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H77" t="n">
@@ -6829,7 +6829,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>16:25 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H78" t="n">
@@ -6911,7 +6911,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Wed, February 4th at 9:00 PM EST</t>
+          <t>17:39 - 2nd Half</t>
         </is>
       </c>
       <c r="H79" t="n">
@@ -6930,7 +6930,7 @@
         <v>0</v>
       </c>
       <c r="M79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N79" t="n">
         <v>0</v>
@@ -6939,19 +6939,19 @@
         <v>0</v>
       </c>
       <c r="P79" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q79" t="n">
         <v>0</v>
       </c>
       <c r="R79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S79" t="n">
         <v>0</v>
       </c>
       <c r="T79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U79" t="n">
         <v>0</v>
@@ -7004,11 +7004,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Boozers Losers</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -7017,11 +7017,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>G-Flop</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -7034,7 +7034,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -7043,37 +7043,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Backslashers</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bend Rimmers</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hilton Heads</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C7" t="n">
         <v>4</v>
@@ -7082,11 +7082,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Three Dawg Nite</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
         <v>4</v>

</xml_diff>